<commit_message>
Excel update and bugfix
</commit_message>
<xml_diff>
--- a/NamingConventionTool/src/main/java/org/openepics/names/ui/devices/NamingImportTemplate.xlsx
+++ b/NamingConventionTool/src/main/java/org/openepics/names/ui/devices/NamingImportTemplate.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Section</t>
   </si>
@@ -32,7 +32,25 @@
     <t>Instance Index</t>
   </si>
   <si>
-    <t>Comment</t>
+    <t>Description/Comment</t>
+  </si>
+  <si>
+    <t>Sec</t>
+  </si>
+  <si>
+    <t>Sub</t>
+  </si>
+  <si>
+    <t>Dis</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>Idx</t>
+  </si>
+  <si>
+    <t>replace this row with real data before uploading. All name elements, except for the instance index, needs to be approved in the Area and Device structrure of the Naming Service before import. </t>
   </si>
 </sst>
 </file>
@@ -151,7 +169,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="F1" activeCellId="0" pane="topLeft" sqref="F1"/>
@@ -160,10 +178,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.6518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.4148148148148"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.2185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.5023255813953"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.646511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.4139534883721"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.506976744186"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11"/>
   </cols>
   <sheetData>
@@ -185,6 +203,26 @@
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>